<commit_message>
Add end decoded pos
</commit_message>
<xml_diff>
--- a/enigma_algorithm.xlsx
+++ b/enigma_algorithm.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dunlapww/turing/mod_1/projects/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dunlapww/turing/mod_1/projects/final_individual/enigma/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{884029C5-653B-A544-9705-D8ACEACCB7F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FE97E13-F8D1-1749-8AE5-EE589FF0EB9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="35880" yWindow="2940" windowWidth="28040" windowHeight="17040" xr2:uid="{1472DCA2-B658-274C-BA6B-193296C9D662}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="66">
   <si>
     <t>date</t>
   </si>
@@ -199,6 +199,39 @@
   </si>
   <si>
     <t>new letter pos</t>
+  </si>
+  <si>
+    <t>final_shifts</t>
+  </si>
+  <si>
+    <t>key letter</t>
+  </si>
+  <si>
+    <t>decode_shift</t>
+  </si>
+  <si>
+    <t>ne letter pos (mod 27)</t>
+  </si>
+  <si>
+    <t>rotate end</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>=</t>
+  </si>
+  <si>
+    <t>-key</t>
+  </si>
+  <si>
+    <t>-offset</t>
+  </si>
+  <si>
+    <t>-correct letter pos</t>
+  </si>
+  <si>
+    <t>multiple of 27</t>
   </si>
 </sst>
 </file>
@@ -222,12 +255,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -247,7 +286,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -562,10 +601,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A197666-CD44-1146-B1F3-7135C7036ABB}">
-  <dimension ref="A1:L50"/>
+  <dimension ref="A1:L60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -583,7 +622,7 @@
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2">
         <f ca="1">RANDBETWEEN(10000,99999)</f>
-        <v>66783</v>
+        <v>43434</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -865,11 +904,11 @@
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C18">
         <f t="shared" ref="C18:C28" si="4">VLOOKUP(B18,$K$10:$L$36,2,FALSE)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D18">
         <f>E10</f>
@@ -877,11 +916,11 @@
       </c>
       <c r="E18">
         <f>MOD(SUM(C18:D18),27)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F18" t="str">
         <f>VLOOKUP(E18,$J$10:$K$36,2,FALSE)</f>
-        <v>j</v>
+        <v>k</v>
       </c>
       <c r="J18">
         <f t="shared" si="3"/>
@@ -900,11 +939,11 @@
         <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="C19">
         <f t="shared" si="4"/>
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="D19">
         <f t="shared" ref="D19:D21" si="5">E11</f>
@@ -912,11 +951,11 @@
       </c>
       <c r="E19">
         <f t="shared" ref="E19:E28" si="6">MOD(SUM(C19:D19),27)</f>
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="F19" t="str">
         <f t="shared" ref="F19:F28" si="7">VLOOKUP(E19,$J$10:$K$36,2,FALSE)</f>
-        <v>o</v>
+        <v>e</v>
       </c>
       <c r="J19">
         <f t="shared" si="3"/>
@@ -935,11 +974,11 @@
         <v>3</v>
       </c>
       <c r="B20" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C20">
         <f t="shared" si="4"/>
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D20">
         <f t="shared" si="5"/>
@@ -947,11 +986,11 @@
       </c>
       <c r="E20">
         <f t="shared" si="6"/>
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F20" t="str">
         <f t="shared" si="7"/>
-        <v>l</v>
+        <v>q</v>
       </c>
       <c r="J20">
         <f t="shared" si="3"/>
@@ -1005,11 +1044,11 @@
         <v>5</v>
       </c>
       <c r="B22" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C22">
         <f t="shared" si="4"/>
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="D22">
         <f>E10</f>
@@ -1017,11 +1056,11 @@
       </c>
       <c r="E22">
         <f t="shared" si="6"/>
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="F22" t="str">
         <f t="shared" si="7"/>
-        <v>v</v>
+        <v>a</v>
       </c>
       <c r="J22">
         <f t="shared" si="3"/>
@@ -1075,11 +1114,11 @@
         <v>7</v>
       </c>
       <c r="B24" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="C24">
         <f t="shared" si="4"/>
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D24">
         <f t="shared" si="8"/>
@@ -1087,11 +1126,11 @@
       </c>
       <c r="E24">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="F24" t="str">
         <f t="shared" si="7"/>
-        <v>e</v>
+        <v>m</v>
       </c>
       <c r="J24">
         <f t="shared" si="3"/>
@@ -1110,11 +1149,11 @@
         <v>8</v>
       </c>
       <c r="B25" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="C25">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="D25">
         <f t="shared" si="8"/>
@@ -1122,11 +1161,11 @@
       </c>
       <c r="E25">
         <f t="shared" si="6"/>
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="F25" t="str">
         <f t="shared" si="7"/>
-        <v>y</v>
+        <v>t</v>
       </c>
       <c r="J25">
         <f t="shared" si="3"/>
@@ -1145,11 +1184,11 @@
         <v>9</v>
       </c>
       <c r="B26" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="C26">
         <f t="shared" si="4"/>
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="D26">
         <f>E10</f>
@@ -1157,11 +1196,11 @@
       </c>
       <c r="E26">
         <f t="shared" si="6"/>
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="F26" t="str">
         <f t="shared" si="7"/>
-        <v>r</v>
+        <v>h</v>
       </c>
       <c r="J26">
         <f t="shared" si="3"/>
@@ -1215,11 +1254,11 @@
         <v>11</v>
       </c>
       <c r="B28" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C28">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D28">
         <f t="shared" si="9"/>
@@ -1227,11 +1266,11 @@
       </c>
       <c r="E28">
         <f t="shared" si="6"/>
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F28" t="str">
         <f t="shared" si="7"/>
-        <v>x</v>
+        <v>w</v>
       </c>
       <c r="J28">
         <f t="shared" si="3"/>
@@ -1445,6 +1484,11 @@
         <v>-20</v>
       </c>
     </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C38" t="s">
+        <v>59</v>
+      </c>
+    </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B39" s="2" t="s">
         <v>49</v>
@@ -1453,12 +1497,30 @@
         <v>44</v>
       </c>
       <c r="D39" t="s">
+        <v>56</v>
+      </c>
+      <c r="E39" t="s">
+        <v>14</v>
+      </c>
+      <c r="F39" t="s">
         <v>5</v>
       </c>
-      <c r="E39" t="s">
+      <c r="G39" t="s">
+        <v>55</v>
+      </c>
+      <c r="H39" t="s">
+        <v>57</v>
+      </c>
+      <c r="I39" t="s">
         <v>54</v>
       </c>
-      <c r="F39" t="s">
+      <c r="J39" t="s">
+        <v>58</v>
+      </c>
+      <c r="K39" t="s">
+        <v>54</v>
+      </c>
+      <c r="L39" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1468,23 +1530,42 @@
       </c>
       <c r="B40" t="str">
         <f>F18</f>
-        <v>j</v>
+        <v>k</v>
       </c>
       <c r="C40">
         <f>VLOOKUP(B40,$K$10:$L$36,2,FALSE)</f>
+        <v>10</v>
+      </c>
+      <c r="D40" t="s">
         <v>9</v>
       </c>
-      <c r="D40">
-        <f>H34</f>
+      <c r="E40" t="str">
+        <f>E34</f>
+        <v>02</v>
+      </c>
+      <c r="F40" t="str">
+        <f>F34</f>
+        <v>1</v>
+      </c>
+      <c r="G40">
+        <f>E40+F40</f>
+        <v>3</v>
+      </c>
+      <c r="H40">
+        <f>-1*G40</f>
         <v>-3</v>
       </c>
-      <c r="E40">
-        <f>MOD(SUM(C40:D40),27)</f>
-        <v>6</v>
-      </c>
-      <c r="F40" t="str">
-        <f>VLOOKUP(E40,$J$10:$K$36,2,FALSE)</f>
-        <v>g</v>
+      <c r="I40">
+        <f>H40+C40</f>
+        <v>7</v>
+      </c>
+      <c r="J40">
+        <f>MOD(I40,27)</f>
+        <v>7</v>
+      </c>
+      <c r="L40" t="str">
+        <f>VLOOKUP(J40,$J$10:$K$36,2,FALSE)</f>
+        <v>h</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
@@ -1493,23 +1574,42 @@
       </c>
       <c r="B41" t="str">
         <f t="shared" ref="B41:B50" si="13">F19</f>
-        <v>o</v>
+        <v>e</v>
       </c>
       <c r="C41">
         <f t="shared" ref="C41:C50" si="14">VLOOKUP(B41,$K$10:$L$36,2,FALSE)</f>
-        <v>14</v>
-      </c>
-      <c r="D41">
-        <f t="shared" ref="D41:D43" si="15">H35</f>
+        <v>4</v>
+      </c>
+      <c r="D41" t="s">
+        <v>10</v>
+      </c>
+      <c r="E41" t="str">
+        <f>E35</f>
+        <v>27</v>
+      </c>
+      <c r="F41" t="str">
+        <f>F35</f>
         <v>0</v>
       </c>
-      <c r="E41">
-        <f t="shared" ref="E41:E50" si="16">MOD(SUM(C41:D41),27)</f>
-        <v>14</v>
-      </c>
-      <c r="F41" t="str">
-        <f t="shared" ref="F41:F50" si="17">VLOOKUP(E41,$J$10:$K$36,2,FALSE)</f>
-        <v>o</v>
+      <c r="G41">
+        <f t="shared" ref="G41:G50" si="15">E41+F41</f>
+        <v>27</v>
+      </c>
+      <c r="H41">
+        <f t="shared" ref="H41:H50" si="16">-1*G41</f>
+        <v>-27</v>
+      </c>
+      <c r="I41">
+        <f t="shared" ref="I41:I50" si="17">H41+C41</f>
+        <v>-23</v>
+      </c>
+      <c r="J41">
+        <f t="shared" ref="J41:J50" si="18">MOD(I41,27)</f>
+        <v>4</v>
+      </c>
+      <c r="L41" t="str">
+        <f t="shared" ref="L41:L50" si="19">VLOOKUP(J41,$J$10:$K$36,2,FALSE)</f>
+        <v>e</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.2">
@@ -1518,23 +1618,42 @@
       </c>
       <c r="B42" t="str">
         <f t="shared" si="13"/>
-        <v>l</v>
+        <v>q</v>
       </c>
       <c r="C42">
         <f t="shared" si="14"/>
+        <v>16</v>
+      </c>
+      <c r="D42" t="s">
         <v>11</v>
       </c>
-      <c r="D42">
+      <c r="E42" t="str">
+        <f>E36</f>
+        <v>71</v>
+      </c>
+      <c r="F42" t="str">
+        <f>F36</f>
+        <v>2</v>
+      </c>
+      <c r="G42">
         <f t="shared" si="15"/>
-        <v>-19</v>
-      </c>
-      <c r="E42">
+        <v>73</v>
+      </c>
+      <c r="H42">
         <f t="shared" si="16"/>
-        <v>19</v>
-      </c>
-      <c r="F42" t="str">
+        <v>-73</v>
+      </c>
+      <c r="I42">
         <f t="shared" si="17"/>
-        <v>t</v>
+        <v>-57</v>
+      </c>
+      <c r="J42">
+        <f t="shared" si="18"/>
+        <v>24</v>
+      </c>
+      <c r="L42" t="str">
+        <f t="shared" si="19"/>
+        <v>y</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.2">
@@ -1549,16 +1668,35 @@
         <f t="shared" si="14"/>
         <v>19</v>
       </c>
-      <c r="D43">
+      <c r="D43" t="s">
+        <v>12</v>
+      </c>
+      <c r="E43" t="str">
+        <f>E37</f>
+        <v>15</v>
+      </c>
+      <c r="F43" t="str">
+        <f>F37</f>
+        <v>5</v>
+      </c>
+      <c r="G43">
         <f t="shared" si="15"/>
+        <v>20</v>
+      </c>
+      <c r="H43">
+        <f t="shared" si="16"/>
         <v>-20</v>
       </c>
-      <c r="E43">
-        <f t="shared" si="16"/>
+      <c r="I43">
+        <f t="shared" si="17"/>
+        <v>-1</v>
+      </c>
+      <c r="J43">
+        <f t="shared" si="18"/>
         <v>26</v>
       </c>
-      <c r="F43" t="str">
-        <f t="shared" si="17"/>
+      <c r="L43" t="str">
+        <f t="shared" si="19"/>
         <v>/</v>
       </c>
     </row>
@@ -1568,23 +1706,42 @@
       </c>
       <c r="B44" t="str">
         <f t="shared" si="13"/>
-        <v>v</v>
+        <v>a</v>
       </c>
       <c r="C44">
         <f t="shared" si="14"/>
-        <v>21</v>
-      </c>
-      <c r="D44" s="4">
-        <f>H34</f>
+        <v>0</v>
+      </c>
+      <c r="D44" t="s">
+        <v>9</v>
+      </c>
+      <c r="E44" t="str">
+        <f>E34</f>
+        <v>02</v>
+      </c>
+      <c r="F44" t="str">
+        <f>F34</f>
+        <v>1</v>
+      </c>
+      <c r="G44">
+        <f t="shared" si="15"/>
+        <v>3</v>
+      </c>
+      <c r="H44">
+        <f t="shared" si="16"/>
         <v>-3</v>
       </c>
-      <c r="E44">
-        <f t="shared" si="16"/>
-        <v>18</v>
-      </c>
-      <c r="F44" t="str">
+      <c r="I44">
         <f t="shared" si="17"/>
-        <v>s</v>
+        <v>-3</v>
+      </c>
+      <c r="J44">
+        <f t="shared" si="18"/>
+        <v>24</v>
+      </c>
+      <c r="L44" t="str">
+        <f t="shared" si="19"/>
+        <v>y</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.2">
@@ -1599,16 +1756,35 @@
         <f t="shared" si="14"/>
         <v>14</v>
       </c>
-      <c r="D45" s="4">
-        <f t="shared" ref="D45:D47" si="18">H35</f>
+      <c r="D45" t="s">
+        <v>10</v>
+      </c>
+      <c r="E45" t="str">
+        <f>E35</f>
+        <v>27</v>
+      </c>
+      <c r="F45" t="str">
+        <f>F35</f>
         <v>0</v>
       </c>
-      <c r="E45">
+      <c r="G45">
+        <f t="shared" si="15"/>
+        <v>27</v>
+      </c>
+      <c r="H45">
         <f t="shared" si="16"/>
+        <v>-27</v>
+      </c>
+      <c r="I45">
+        <f t="shared" si="17"/>
+        <v>-13</v>
+      </c>
+      <c r="J45">
+        <f t="shared" si="18"/>
         <v>14</v>
       </c>
-      <c r="F45" t="str">
-        <f t="shared" si="17"/>
+      <c r="L45" t="str">
+        <f t="shared" si="19"/>
         <v>o</v>
       </c>
     </row>
@@ -1618,23 +1794,42 @@
       </c>
       <c r="B46" t="str">
         <f t="shared" si="13"/>
-        <v>e</v>
+        <v>m</v>
       </c>
       <c r="C46">
         <f t="shared" si="14"/>
-        <v>4</v>
-      </c>
-      <c r="D46" s="4">
+        <v>12</v>
+      </c>
+      <c r="D46" t="s">
+        <v>11</v>
+      </c>
+      <c r="E46" t="str">
+        <f>E36</f>
+        <v>71</v>
+      </c>
+      <c r="F46" t="str">
+        <f>F36</f>
+        <v>2</v>
+      </c>
+      <c r="G46">
+        <f t="shared" si="15"/>
+        <v>73</v>
+      </c>
+      <c r="H46">
+        <f t="shared" si="16"/>
+        <v>-73</v>
+      </c>
+      <c r="I46">
+        <f t="shared" si="17"/>
+        <v>-61</v>
+      </c>
+      <c r="J46">
         <f t="shared" si="18"/>
-        <v>-19</v>
-      </c>
-      <c r="E46">
-        <f t="shared" si="16"/>
-        <v>12</v>
-      </c>
-      <c r="F46" t="str">
-        <f t="shared" si="17"/>
-        <v>m</v>
+        <v>20</v>
+      </c>
+      <c r="L46" t="str">
+        <f t="shared" si="19"/>
+        <v>u</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.2">
@@ -1643,23 +1838,42 @@
       </c>
       <c r="B47" t="str">
         <f t="shared" si="13"/>
-        <v>y</v>
+        <v>t</v>
       </c>
       <c r="C47">
         <f t="shared" si="14"/>
-        <v>24</v>
-      </c>
-      <c r="D47" s="4">
+        <v>19</v>
+      </c>
+      <c r="D47" t="s">
+        <v>12</v>
+      </c>
+      <c r="E47" t="str">
+        <f>E37</f>
+        <v>15</v>
+      </c>
+      <c r="F47" t="str">
+        <f>F37</f>
+        <v>5</v>
+      </c>
+      <c r="G47">
+        <f t="shared" si="15"/>
+        <v>20</v>
+      </c>
+      <c r="H47">
+        <f t="shared" si="16"/>
+        <v>-20</v>
+      </c>
+      <c r="I47">
+        <f t="shared" si="17"/>
+        <v>-1</v>
+      </c>
+      <c r="J47">
         <f t="shared" si="18"/>
-        <v>-20</v>
-      </c>
-      <c r="E47">
-        <f t="shared" si="16"/>
-        <v>4</v>
-      </c>
-      <c r="F47" t="str">
-        <f t="shared" si="17"/>
-        <v>e</v>
+        <v>26</v>
+      </c>
+      <c r="L47" t="str">
+        <f t="shared" si="19"/>
+        <v>/</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.2">
@@ -1668,26 +1882,45 @@
       </c>
       <c r="B48" t="str">
         <f t="shared" si="13"/>
-        <v>r</v>
+        <v>h</v>
       </c>
       <c r="C48">
         <f t="shared" si="14"/>
-        <v>17</v>
-      </c>
-      <c r="D48" s="4">
-        <f>H34</f>
+        <v>7</v>
+      </c>
+      <c r="D48" t="s">
+        <v>9</v>
+      </c>
+      <c r="E48" s="4" t="str">
+        <f>E34</f>
+        <v>02</v>
+      </c>
+      <c r="F48" t="str">
+        <f>F34</f>
+        <v>1</v>
+      </c>
+      <c r="G48">
+        <f t="shared" si="15"/>
+        <v>3</v>
+      </c>
+      <c r="H48">
+        <f t="shared" si="16"/>
         <v>-3</v>
       </c>
-      <c r="E48">
-        <f t="shared" si="16"/>
-        <v>14</v>
-      </c>
-      <c r="F48" t="str">
+      <c r="I48">
         <f t="shared" si="17"/>
-        <v>o</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+      <c r="J48">
+        <f t="shared" si="18"/>
+        <v>4</v>
+      </c>
+      <c r="L48" t="str">
+        <f t="shared" si="19"/>
+        <v>e</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>10</v>
       </c>
@@ -1699,42 +1932,211 @@
         <f t="shared" si="14"/>
         <v>13</v>
       </c>
-      <c r="D49" s="4">
-        <f t="shared" ref="D49:D50" si="19">H35</f>
+      <c r="D49" t="s">
+        <v>10</v>
+      </c>
+      <c r="E49" t="str">
+        <f>E35</f>
+        <v>27</v>
+      </c>
+      <c r="F49" t="str">
+        <f>F35</f>
         <v>0</v>
       </c>
-      <c r="E49">
+      <c r="G49">
+        <f t="shared" si="15"/>
+        <v>27</v>
+      </c>
+      <c r="H49">
         <f t="shared" si="16"/>
+        <v>-27</v>
+      </c>
+      <c r="I49">
+        <f t="shared" si="17"/>
+        <v>-14</v>
+      </c>
+      <c r="J49">
+        <f t="shared" si="18"/>
         <v>13</v>
       </c>
-      <c r="F49" t="str">
-        <f t="shared" si="17"/>
+      <c r="L49" t="str">
+        <f t="shared" si="19"/>
         <v>n</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>11</v>
       </c>
       <c r="B50" t="str">
         <f t="shared" si="13"/>
-        <v>x</v>
+        <v>w</v>
       </c>
       <c r="C50">
         <f t="shared" si="14"/>
-        <v>23</v>
-      </c>
-      <c r="D50" s="4">
+        <v>22</v>
+      </c>
+      <c r="D50" t="s">
+        <v>11</v>
+      </c>
+      <c r="E50" t="str">
+        <f>E36</f>
+        <v>71</v>
+      </c>
+      <c r="F50" t="str">
+        <f>F36</f>
+        <v>2</v>
+      </c>
+      <c r="G50">
+        <f t="shared" si="15"/>
+        <v>73</v>
+      </c>
+      <c r="H50">
+        <f t="shared" si="16"/>
+        <v>-73</v>
+      </c>
+      <c r="I50">
+        <f t="shared" si="17"/>
+        <v>-51</v>
+      </c>
+      <c r="J50">
+        <f t="shared" si="18"/>
+        <v>3</v>
+      </c>
+      <c r="L50" t="str">
         <f t="shared" si="19"/>
-        <v>-19</v>
-      </c>
-      <c r="E50">
-        <f t="shared" si="16"/>
+        <v>d</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C53">
+        <v>7</v>
+      </c>
+      <c r="E53" t="s">
+        <v>60</v>
+      </c>
+      <c r="F53">
+        <v>-1</v>
+      </c>
+      <c r="H53" t="s">
+        <v>61</v>
+      </c>
+      <c r="I53">
+        <v>0</v>
+      </c>
+      <c r="J53">
+        <v>0</v>
+      </c>
+      <c r="L53">
         <v>4</v>
       </c>
-      <c r="F50" t="str">
-        <f t="shared" si="17"/>
-        <v>e</v>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C54">
+        <v>7</v>
+      </c>
+      <c r="E54" t="s">
+        <v>60</v>
+      </c>
+      <c r="F54">
+        <v>-1</v>
+      </c>
+      <c r="H54" t="s">
+        <v>61</v>
+      </c>
+      <c r="I54">
+        <f>J54*27</f>
+        <v>27</v>
+      </c>
+      <c r="J54">
+        <f>J53+1</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C55">
+        <v>7</v>
+      </c>
+      <c r="E55" t="s">
+        <v>60</v>
+      </c>
+      <c r="F55">
+        <v>-1</v>
+      </c>
+      <c r="H55" t="s">
+        <v>61</v>
+      </c>
+      <c r="I55">
+        <f t="shared" ref="I55:I59" si="20">J55*27</f>
+        <v>54</v>
+      </c>
+      <c r="J55">
+        <f t="shared" ref="J55:J57" si="21">J54+1</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C56">
+        <v>7</v>
+      </c>
+      <c r="E56" t="s">
+        <v>60</v>
+      </c>
+      <c r="F56">
+        <v>-1</v>
+      </c>
+      <c r="H56" t="s">
+        <v>61</v>
+      </c>
+      <c r="I56">
+        <f t="shared" si="20"/>
+        <v>81</v>
+      </c>
+      <c r="J56">
+        <f t="shared" si="21"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C57">
+        <v>7</v>
+      </c>
+      <c r="E57" t="s">
+        <v>60</v>
+      </c>
+      <c r="F57">
+        <v>-1</v>
+      </c>
+      <c r="H57" t="s">
+        <v>61</v>
+      </c>
+      <c r="I57">
+        <f t="shared" si="20"/>
+        <v>108</v>
+      </c>
+      <c r="J57">
+        <f t="shared" si="21"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C60" t="s">
+        <v>44</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F60" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="H60" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="J60" t="s">
+        <v>61</v>
+      </c>
+      <c r="K60" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>